<commit_message>
Have added some more reporting and minor alterations to other functionality
</commit_message>
<xml_diff>
--- a/data/input/test_scripts_1/A.xlsx
+++ b/data/input/test_scripts_1/A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\workspace\modules\data_curation\data\input\test_scripts_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1391B33-47FA-4930-B190-2EF4DC28706E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CD9CB0-B02A-4351-B42B-6F3319121895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A83F083F-E720-4BC0-9660-EB89CD7A1A69}"/>
+    <workbookView xWindow="3760" yWindow="2790" windowWidth="16920" windowHeight="10540" xr2:uid="{A83F083F-E720-4BC0-9660-EB89CD7A1A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Number</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Pho</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A69BA486-D3B4-411D-A620-1F82B1AC555A}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -436,7 +442,7 @@
     <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +455,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,8 +475,14 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>51.507399999999997</v>
+      </c>
+      <c r="F2">
+        <v>0.1278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -477,8 +495,16 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <f>E2+0.001</f>
+        <v>51.508399999999995</v>
+      </c>
+      <c r="F3">
+        <f>F2-0.001</f>
+        <v>0.1268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -491,8 +517,16 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <f t="shared" ref="E4:E12" si="0">E3+0.001</f>
+        <v>51.509399999999992</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F12" si="1">F3-0.001</f>
+        <v>0.1258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -505,8 +539,16 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>51.51039999999999</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.12479999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -516,8 +558,16 @@
       <c r="C6" s="1">
         <v>42932</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>51.511399999999988</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.12379999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -527,8 +577,16 @@
       <c r="C7" s="1">
         <v>42843</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>51.512399999999985</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.12279999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -541,8 +599,16 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>51.513399999999983</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.12179999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -555,8 +621,16 @@
       <c r="D9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>51.514399999999981</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.12079999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1234</v>
       </c>
@@ -569,8 +643,16 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>51.515399999999978</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.11979999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -583,8 +665,16 @@
       <c r="D11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>51.516399999999976</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.11879999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2341243</v>
       </c>
@@ -597,8 +687,17 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>51.517399999999974</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.11779999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Further development, looked mostly at extending the examples
</commit_message>
<xml_diff>
--- a/data/input/test_scripts_1/A.xlsx
+++ b/data/input/test_scripts_1/A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\workspace\modules\data_curation\data\input\test_scripts_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CD9CB0-B02A-4351-B42B-6F3319121895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AA191C-C2B5-48DE-9145-1FAB32348BD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="2790" windowWidth="16920" windowHeight="10540" xr2:uid="{A83F083F-E720-4BC0-9660-EB89CD7A1A69}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A83F083F-E720-4BC0-9660-EB89CD7A1A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,13 +431,13 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>